<commit_message>
updates to export of L144
</commit_message>
<xml_diff>
--- a/exports/L144-tok-result-csv.xlsx
+++ b/exports/L144-tok-result-csv.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackbowers/Box Sync/Language_Data/Mixtepec_Mixtec/exports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A446575B-0BDC-854A-9E13-AEA7AB60AE2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D300DE-073D-D84A-8FCF-3742FF4D797D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2900" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{F22C7306-1053-6340-BDEB-87E227009965}"/>
+    <workbookView xWindow="2860" yWindow="620" windowWidth="28040" windowHeight="17040" xr2:uid="{F22C7306-1053-6340-BDEB-87E227009965}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="L144_tok_result_csv" localSheetId="0">Sheet1!$A$1:$P$213</definedName>
+    <definedName name="L144_tok_result_csv" localSheetId="0">Sheet1!$A$1:$P$202</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="487">
   <si>
     <t>Orth</t>
   </si>
@@ -1411,15 +1411,6 @@
   </si>
   <si>
     <t>corn drink</t>
-  </si>
-  <si>
-    <t>utsi</t>
-  </si>
-  <si>
-    <t>ten</t>
-  </si>
-  <si>
-    <t>diez</t>
   </si>
   <si>
     <t>uvia</t>
@@ -1898,10 +1889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B3E7DB-1E03-3045-A456-355D83C6CA68}">
-  <dimension ref="A1:O213"/>
+  <dimension ref="A1:O202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:XFD46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2741,43 +2732,43 @@
         <v>175</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="46" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H46" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="M46" t="s">
+      <c r="M46" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="N46" t="s">
+      <c r="N46" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="O46" t="s">
+      <c r="O46" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="47" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H47" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="M47" t="s">
+      <c r="M47" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="N47" t="s">
+      <c r="N47" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="O47" t="s">
+      <c r="O47" s="1" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3144,7 +3135,7 @@
         <v>31</v>
       </c>
       <c r="M68" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="N68" t="s">
         <v>19</v>
@@ -3351,7 +3342,7 @@
         <v>290</v>
       </c>
       <c r="M77" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="N77" t="s">
         <v>19</v>
@@ -3478,23 +3469,23 @@
         <v>118</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+    <row r="83" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E83" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="H83" t="s">
+      <c r="H83" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="M83" t="s">
+      <c r="M83" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="N83" t="s">
+      <c r="N83" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="O83" t="s">
+      <c r="O83" s="1" t="s">
         <v>93</v>
       </c>
     </row>
@@ -3520,7 +3511,10 @@
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>46</v>
+        <v>306</v>
+      </c>
+      <c r="C85" t="s">
+        <v>307</v>
       </c>
       <c r="E85" t="s">
         <v>296</v>
@@ -3529,13 +3523,13 @@
         <v>255</v>
       </c>
       <c r="M85" t="s">
-        <v>297</v>
+        <v>57</v>
       </c>
       <c r="N85" t="s">
-        <v>298</v>
+        <v>58</v>
       </c>
       <c r="O85" t="s">
-        <v>299</v>
+        <v>59</v>
       </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.2">
@@ -3549,213 +3543,219 @@
         <v>255</v>
       </c>
       <c r="M86" t="s">
-        <v>300</v>
+        <v>127</v>
       </c>
       <c r="N86" t="s">
-        <v>301</v>
+        <v>128</v>
       </c>
       <c r="O86" t="s">
-        <v>302</v>
+        <v>129</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>46</v>
+        <v>308</v>
       </c>
       <c r="E87" t="s">
-        <v>296</v>
+        <v>309</v>
       </c>
       <c r="H87" t="s">
-        <v>255</v>
+        <v>310</v>
       </c>
       <c r="M87" t="s">
-        <v>303</v>
+        <v>91</v>
       </c>
       <c r="N87" t="s">
-        <v>304</v>
+        <v>92</v>
       </c>
       <c r="O87" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>306</v>
-      </c>
-      <c r="C88" t="s">
-        <v>307</v>
-      </c>
-      <c r="E88" t="s">
-        <v>296</v>
-      </c>
-      <c r="H88" t="s">
-        <v>255</v>
-      </c>
-      <c r="M88" t="s">
-        <v>57</v>
-      </c>
-      <c r="N88" t="s">
-        <v>58</v>
-      </c>
-      <c r="O88" t="s">
-        <v>59</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="I88" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="J88" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="M88" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="N88" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="O88" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>46</v>
+        <v>318</v>
       </c>
       <c r="E89" t="s">
-        <v>296</v>
+        <v>319</v>
+      </c>
+      <c r="F89" t="s">
+        <v>320</v>
       </c>
       <c r="H89" t="s">
-        <v>255</v>
+        <v>321</v>
       </c>
       <c r="M89" t="s">
-        <v>127</v>
+        <v>79</v>
       </c>
       <c r="N89" t="s">
-        <v>128</v>
+        <v>80</v>
       </c>
       <c r="O89" t="s">
-        <v>129</v>
+        <v>81</v>
       </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>308</v>
+        <v>318</v>
       </c>
       <c r="E90" t="s">
-        <v>309</v>
+        <v>322</v>
       </c>
       <c r="H90" t="s">
-        <v>310</v>
+        <v>323</v>
       </c>
       <c r="M90" t="s">
-        <v>91</v>
-      </c>
-      <c r="N90" t="s">
-        <v>92</v>
-      </c>
-      <c r="O90" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="91" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="H91" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="I91" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="J91" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="M91" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="N91" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O91" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>318</v>
-      </c>
-      <c r="E92" t="s">
-        <v>319</v>
-      </c>
-      <c r="F92" t="s">
-        <v>320</v>
-      </c>
-      <c r="H92" t="s">
-        <v>321</v>
-      </c>
-      <c r="M92" t="s">
-        <v>79</v>
-      </c>
-      <c r="N92" t="s">
-        <v>80</v>
-      </c>
-      <c r="O92" t="s">
-        <v>81</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>324</v>
+      </c>
+      <c r="E91" t="s">
+        <v>325</v>
+      </c>
+      <c r="H91" t="s">
+        <v>326</v>
+      </c>
+      <c r="M91" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M92" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N92" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O92" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
       <c r="E93" t="s">
-        <v>322</v>
+        <v>256</v>
       </c>
       <c r="H93" t="s">
-        <v>323</v>
+        <v>257</v>
       </c>
       <c r="M93" t="s">
-        <v>32</v>
+        <v>486</v>
+      </c>
+      <c r="N93" t="s">
+        <v>19</v>
+      </c>
+      <c r="O93" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>324</v>
+        <v>306</v>
+      </c>
+      <c r="C94" t="s">
+        <v>307</v>
       </c>
       <c r="E94" t="s">
-        <v>325</v>
+        <v>296</v>
       </c>
       <c r="H94" t="s">
-        <v>326</v>
+        <v>255</v>
       </c>
       <c r="M94" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="95" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="H95" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="M95" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N94" t="s">
+        <v>58</v>
+      </c>
+      <c r="O94" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>330</v>
+      </c>
+      <c r="E95" t="s">
+        <v>331</v>
+      </c>
+      <c r="H95" t="s">
+        <v>332</v>
+      </c>
+      <c r="M95" t="s">
         <v>40</v>
       </c>
-      <c r="N95" s="1" t="s">
+      <c r="N95" t="s">
         <v>41</v>
       </c>
-      <c r="O95" s="1" t="s">
+      <c r="O95" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="E96" t="s">
-        <v>256</v>
+        <v>287</v>
+      </c>
+      <c r="F96" t="s">
+        <v>288</v>
       </c>
       <c r="H96" t="s">
-        <v>257</v>
+        <v>289</v>
+      </c>
+      <c r="I96" t="s">
+        <v>290</v>
       </c>
       <c r="M96" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="N96" t="s">
         <v>19</v>
@@ -3766,91 +3766,82 @@
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>306</v>
-      </c>
-      <c r="C97" t="s">
-        <v>307</v>
+        <v>238</v>
       </c>
       <c r="E97" t="s">
-        <v>296</v>
+        <v>239</v>
       </c>
       <c r="H97" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="M97" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="N97" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="O97" t="s">
-        <v>59</v>
+        <v>102</v>
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>330</v>
+        <v>238</v>
       </c>
       <c r="E98" t="s">
-        <v>331</v>
+        <v>74</v>
       </c>
       <c r="H98" t="s">
-        <v>332</v>
+        <v>75</v>
       </c>
       <c r="M98" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="N98" t="s">
-        <v>41</v>
+        <v>104</v>
       </c>
       <c r="O98" t="s">
-        <v>42</v>
+        <v>105</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>286</v>
+        <v>238</v>
       </c>
       <c r="E99" t="s">
-        <v>287</v>
-      </c>
-      <c r="F99" t="s">
-        <v>288</v>
+        <v>74</v>
       </c>
       <c r="H99" t="s">
-        <v>289</v>
-      </c>
-      <c r="I99" t="s">
-        <v>290</v>
+        <v>75</v>
       </c>
       <c r="M99" t="s">
-        <v>489</v>
+        <v>79</v>
       </c>
       <c r="N99" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="O99" t="s">
-        <v>20</v>
+        <v>81</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>238</v>
+        <v>330</v>
       </c>
       <c r="E100" t="s">
-        <v>239</v>
+        <v>331</v>
       </c>
       <c r="H100" t="s">
-        <v>240</v>
+        <v>332</v>
       </c>
       <c r="M100" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="N100" t="s">
-        <v>101</v>
+        <v>41</v>
       </c>
       <c r="O100" t="s">
-        <v>102</v>
+        <v>42</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.2">
@@ -3864,228 +3855,228 @@
         <v>75</v>
       </c>
       <c r="M101" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="N101" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="O101" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>238</v>
-      </c>
-      <c r="E102" t="s">
-        <v>74</v>
-      </c>
-      <c r="H102" t="s">
-        <v>75</v>
-      </c>
-      <c r="M102" t="s">
-        <v>79</v>
-      </c>
-      <c r="N102" t="s">
-        <v>80</v>
-      </c>
-      <c r="O102" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>330</v>
-      </c>
-      <c r="E103" t="s">
-        <v>331</v>
-      </c>
-      <c r="H103" t="s">
-        <v>332</v>
-      </c>
-      <c r="M103" t="s">
-        <v>40</v>
-      </c>
-      <c r="N103" t="s">
-        <v>41</v>
-      </c>
-      <c r="O103" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>238</v>
-      </c>
-      <c r="E104" t="s">
-        <v>74</v>
-      </c>
-      <c r="H104" t="s">
-        <v>75</v>
-      </c>
-      <c r="M104" t="s">
-        <v>106</v>
-      </c>
-      <c r="N104" t="s">
-        <v>107</v>
-      </c>
-      <c r="O104" t="s">
-        <v>108</v>
+        <v>22</v>
+      </c>
+      <c r="B104" t="s">
+        <v>23</v>
+      </c>
+      <c r="C104" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>17</v>
+        <v>238</v>
+      </c>
+      <c r="E105" t="s">
+        <v>239</v>
+      </c>
+      <c r="H105" t="s">
+        <v>242</v>
+      </c>
+      <c r="M105" t="s">
+        <v>486</v>
+      </c>
+      <c r="N105" t="s">
+        <v>19</v>
+      </c>
+      <c r="O105" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>18</v>
+        <v>238</v>
+      </c>
+      <c r="E106" t="s">
+        <v>74</v>
+      </c>
+      <c r="H106" t="s">
+        <v>75</v>
+      </c>
+      <c r="M106" t="s">
+        <v>119</v>
+      </c>
+      <c r="N106" t="s">
+        <v>120</v>
+      </c>
+      <c r="O106" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>22</v>
-      </c>
-      <c r="B107" t="s">
-        <v>23</v>
-      </c>
-      <c r="C107" t="s">
-        <v>24</v>
+        <v>333</v>
+      </c>
+      <c r="E107" t="s">
+        <v>334</v>
+      </c>
+      <c r="H107" t="s">
+        <v>335</v>
+      </c>
+      <c r="M107" t="s">
+        <v>91</v>
+      </c>
+      <c r="N107" t="s">
+        <v>92</v>
+      </c>
+      <c r="O107" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>238</v>
+        <v>333</v>
       </c>
       <c r="E108" t="s">
-        <v>239</v>
+        <v>334</v>
       </c>
       <c r="H108" t="s">
-        <v>242</v>
+        <v>335</v>
       </c>
       <c r="M108" t="s">
-        <v>489</v>
+        <v>94</v>
       </c>
       <c r="N108" t="s">
-        <v>19</v>
+        <v>95</v>
       </c>
       <c r="O108" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>238</v>
+        <v>342</v>
       </c>
       <c r="E109" t="s">
-        <v>74</v>
+        <v>343</v>
       </c>
       <c r="H109" t="s">
-        <v>75</v>
+        <v>344</v>
       </c>
       <c r="M109" t="s">
-        <v>119</v>
-      </c>
-      <c r="N109" t="s">
-        <v>120</v>
-      </c>
-      <c r="O109" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
-        <v>333</v>
-      </c>
-      <c r="E110" t="s">
-        <v>334</v>
-      </c>
-      <c r="H110" t="s">
-        <v>335</v>
-      </c>
-      <c r="M110" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="M110" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="N110" t="s">
+      <c r="N110" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="O110" t="s">
+      <c r="O110" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>333</v>
+        <v>348</v>
       </c>
       <c r="E111" t="s">
-        <v>334</v>
+        <v>349</v>
       </c>
       <c r="H111" t="s">
-        <v>335</v>
+        <v>350</v>
       </c>
       <c r="M111" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="N111" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="O111" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="E112" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="H112" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="M112" t="s">
-        <v>54</v>
+        <v>149</v>
+      </c>
+      <c r="N112" t="s">
+        <v>150</v>
+      </c>
+      <c r="O112" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="E113" t="s">
-        <v>346</v>
+        <v>354</v>
       </c>
       <c r="H113" t="s">
-        <v>347</v>
+        <v>355</v>
       </c>
       <c r="M113" t="s">
-        <v>91</v>
+        <v>152</v>
       </c>
       <c r="N113" t="s">
-        <v>92</v>
+        <v>153</v>
       </c>
       <c r="O113" t="s">
-        <v>93</v>
+        <v>154</v>
       </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="E114" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
       <c r="H114" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="M114" t="s">
-        <v>91</v>
+        <v>158</v>
       </c>
       <c r="N114" t="s">
-        <v>92</v>
+        <v>159</v>
       </c>
       <c r="O114" t="s">
-        <v>93</v>
+        <v>160</v>
       </c>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.2">
@@ -4093,19 +4084,19 @@
         <v>351</v>
       </c>
       <c r="E115" t="s">
-        <v>352</v>
+        <v>213</v>
       </c>
       <c r="H115" t="s">
-        <v>353</v>
+        <v>212</v>
       </c>
       <c r="M115" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="N115" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="O115" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.2">
@@ -4113,19 +4104,19 @@
         <v>351</v>
       </c>
       <c r="E116" t="s">
-        <v>354</v>
+        <v>211</v>
       </c>
       <c r="H116" t="s">
-        <v>355</v>
+        <v>212</v>
       </c>
       <c r="M116" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="N116" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
       <c r="O116" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.2">
@@ -4133,19 +4124,19 @@
         <v>351</v>
       </c>
       <c r="E117" t="s">
-        <v>356</v>
+        <v>213</v>
       </c>
       <c r="H117" t="s">
-        <v>357</v>
+        <v>212</v>
       </c>
       <c r="M117" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="N117" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="O117" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.2">
@@ -4159,212 +4150,212 @@
         <v>212</v>
       </c>
       <c r="M118" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="N118" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="O118" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="E119" t="s">
-        <v>211</v>
+        <v>359</v>
       </c>
       <c r="H119" t="s">
-        <v>212</v>
+        <v>360</v>
       </c>
       <c r="M119" t="s">
-        <v>167</v>
+        <v>68</v>
       </c>
       <c r="N119" t="s">
-        <v>168</v>
+        <v>69</v>
       </c>
       <c r="O119" t="s">
-        <v>169</v>
+        <v>70</v>
       </c>
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>351</v>
+        <v>361</v>
       </c>
       <c r="E120" t="s">
-        <v>213</v>
+        <v>362</v>
       </c>
       <c r="H120" t="s">
-        <v>212</v>
+        <v>363</v>
       </c>
       <c r="M120" t="s">
-        <v>173</v>
+        <v>63</v>
       </c>
       <c r="N120" t="s">
-        <v>174</v>
+        <v>64</v>
       </c>
       <c r="O120" t="s">
-        <v>175</v>
+        <v>65</v>
       </c>
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>351</v>
+        <v>364</v>
       </c>
       <c r="E121" t="s">
-        <v>213</v>
+        <v>365</v>
       </c>
       <c r="H121" t="s">
-        <v>212</v>
+        <v>366</v>
       </c>
       <c r="M121" t="s">
-        <v>179</v>
+        <v>91</v>
       </c>
       <c r="N121" t="s">
-        <v>180</v>
+        <v>92</v>
       </c>
       <c r="O121" t="s">
-        <v>181</v>
+        <v>93</v>
       </c>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="E122" t="s">
-        <v>359</v>
+        <v>367</v>
       </c>
       <c r="H122" t="s">
-        <v>360</v>
+        <v>368</v>
       </c>
       <c r="M122" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="N122" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="O122" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>361</v>
+        <v>369</v>
       </c>
       <c r="E123" t="s">
-        <v>362</v>
+        <v>209</v>
       </c>
       <c r="H123" t="s">
-        <v>363</v>
+        <v>209</v>
       </c>
       <c r="M123" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="N123" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="O123" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="E124" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="H124" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="M124" t="s">
-        <v>91</v>
-      </c>
-      <c r="N124" t="s">
-        <v>92</v>
-      </c>
-      <c r="O124" t="s">
-        <v>93</v>
+        <v>145</v>
       </c>
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
       <c r="E125" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="H125" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
       <c r="M125" t="s">
-        <v>91</v>
-      </c>
-      <c r="N125" t="s">
-        <v>92</v>
-      </c>
-      <c r="O125" t="s">
-        <v>93</v>
+        <v>51</v>
       </c>
     </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="E126" t="s">
-        <v>209</v>
+        <v>377</v>
       </c>
       <c r="H126" t="s">
-        <v>209</v>
+        <v>378</v>
       </c>
       <c r="M126" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="N126" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="O126" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
     </row>
     <row r="127" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="E127" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="H127" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="M127" t="s">
-        <v>145</v>
+        <v>91</v>
+      </c>
+      <c r="N127" t="s">
+        <v>92</v>
+      </c>
+      <c r="O127" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="E128" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="H128" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="M128" t="s">
-        <v>51</v>
+        <v>106</v>
+      </c>
+      <c r="N128" t="s">
+        <v>107</v>
+      </c>
+      <c r="O128" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="129" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="E129" t="s">
-        <v>377</v>
+        <v>259</v>
       </c>
       <c r="H129" t="s">
-        <v>378</v>
+        <v>260</v>
       </c>
       <c r="M129" t="s">
         <v>91</v>
@@ -4378,156 +4369,150 @@
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="E130" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="H130" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="M130" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="N130" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="O130" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
     </row>
     <row r="131" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="E131" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="H131" t="s">
-        <v>381</v>
+        <v>386</v>
       </c>
       <c r="M131" t="s">
-        <v>106</v>
+        <v>179</v>
       </c>
       <c r="N131" t="s">
-        <v>107</v>
+        <v>180</v>
       </c>
       <c r="O131" t="s">
-        <v>108</v>
+        <v>181</v>
       </c>
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="E132" t="s">
-        <v>259</v>
+        <v>387</v>
       </c>
       <c r="H132" t="s">
-        <v>260</v>
+        <v>388</v>
       </c>
       <c r="M132" t="s">
-        <v>91</v>
-      </c>
-      <c r="N132" t="s">
-        <v>92</v>
-      </c>
-      <c r="O132" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
-        <v>382</v>
-      </c>
-      <c r="E133" t="s">
-        <v>383</v>
-      </c>
-      <c r="H133" t="s">
-        <v>382</v>
-      </c>
-      <c r="M133" t="s">
-        <v>79</v>
-      </c>
-      <c r="N133" t="s">
-        <v>80</v>
-      </c>
-      <c r="O133" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="E134" t="s">
-        <v>385</v>
-      </c>
-      <c r="H134" t="s">
-        <v>386</v>
-      </c>
-      <c r="M134" t="s">
-        <v>179</v>
-      </c>
-      <c r="N134" t="s">
-        <v>180</v>
-      </c>
-      <c r="O134" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
-        <v>384</v>
-      </c>
-      <c r="E135" t="s">
-        <v>387</v>
-      </c>
-      <c r="H135" t="s">
-        <v>388</v>
-      </c>
-      <c r="M135" t="s">
+      <c r="E133" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="H133" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="M133" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
-        <v>384</v>
-      </c>
-      <c r="E136" t="s">
-        <v>389</v>
-      </c>
-      <c r="H136" t="s">
-        <v>390</v>
-      </c>
-      <c r="M136" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A137" t="s">
+    <row r="134" spans="1:15" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="E137" t="s">
+      <c r="E134" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="F137" t="s">
+      <c r="F134" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="H137" t="s">
+      <c r="H134" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="I137" t="s">
+      <c r="I134" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="M137" t="s">
+      <c r="M134" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="N137" t="s">
+      <c r="N134" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="O137" t="s">
+      <c r="O134" s="1" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="H135" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="M135" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="N135" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O135" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="H136" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="M136" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="H137" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="M137" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="N137" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="O137" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="138" spans="1:15" x14ac:dyDescent="0.2">
@@ -4535,19 +4520,19 @@
         <v>391</v>
       </c>
       <c r="E138" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="H138" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="M138" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="N138" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="O138" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
     </row>
     <row r="139" spans="1:15" x14ac:dyDescent="0.2">
@@ -4555,421 +4540,415 @@
         <v>391</v>
       </c>
       <c r="E139" t="s">
-        <v>394</v>
+        <v>205</v>
+      </c>
+      <c r="F139" t="s">
+        <v>312</v>
       </c>
       <c r="H139" t="s">
-        <v>395</v>
+        <v>399</v>
+      </c>
+      <c r="I139" t="s">
+        <v>315</v>
       </c>
       <c r="M139" t="s">
-        <v>21</v>
+        <v>94</v>
+      </c>
+      <c r="N139" t="s">
+        <v>95</v>
+      </c>
+      <c r="O139" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="140" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
       <c r="E140" t="s">
-        <v>394</v>
+        <v>401</v>
       </c>
       <c r="H140" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="M140" t="s">
-        <v>119</v>
+        <v>261</v>
       </c>
       <c r="N140" t="s">
-        <v>120</v>
+        <v>262</v>
       </c>
       <c r="O140" t="s">
-        <v>121</v>
+        <v>263</v>
       </c>
     </row>
     <row r="141" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>391</v>
+        <v>403</v>
       </c>
       <c r="E141" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="H141" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
       <c r="M141" t="s">
-        <v>91</v>
-      </c>
-      <c r="N141" t="s">
-        <v>92</v>
-      </c>
-      <c r="O141" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
-        <v>391</v>
-      </c>
-      <c r="E142" t="s">
-        <v>205</v>
-      </c>
-      <c r="F142" t="s">
-        <v>312</v>
-      </c>
-      <c r="H142" t="s">
-        <v>399</v>
-      </c>
-      <c r="I142" t="s">
-        <v>315</v>
-      </c>
-      <c r="M142" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="H142" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="M142" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="H143" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="M143" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="N143" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="O143" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="H144" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="I144" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="M144" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="N144" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O144" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>410</v>
+      </c>
+      <c r="E145" t="s">
+        <v>411</v>
+      </c>
+      <c r="H145" t="s">
+        <v>412</v>
+      </c>
+      <c r="M145" t="s">
+        <v>79</v>
+      </c>
+      <c r="N145" t="s">
+        <v>80</v>
+      </c>
+      <c r="O145" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>413</v>
+      </c>
+      <c r="E146" t="s">
+        <v>186</v>
+      </c>
+      <c r="H146" t="s">
+        <v>416</v>
+      </c>
+      <c r="M146" t="s">
         <v>94</v>
       </c>
-      <c r="N142" t="s">
+      <c r="N146" t="s">
         <v>95</v>
       </c>
-      <c r="O142" t="s">
+      <c r="O146" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
-        <v>400</v>
-      </c>
-      <c r="E143" t="s">
-        <v>401</v>
-      </c>
-      <c r="H143" t="s">
-        <v>402</v>
-      </c>
-      <c r="M143" t="s">
-        <v>261</v>
-      </c>
-      <c r="N143" t="s">
-        <v>262</v>
-      </c>
-      <c r="O143" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
-        <v>403</v>
-      </c>
-      <c r="E144" t="s">
-        <v>404</v>
-      </c>
-      <c r="H144" t="s">
-        <v>405</v>
-      </c>
-      <c r="M144" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="145" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="E145" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="H145" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="M145" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="146" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="H146" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="M146" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="N146" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="O146" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
-        <v>279</v>
-      </c>
-      <c r="E147" t="s">
-        <v>280</v>
-      </c>
-      <c r="H147" t="s">
-        <v>281</v>
-      </c>
-      <c r="I147" t="s">
-        <v>282</v>
-      </c>
-      <c r="M147" t="s">
-        <v>109</v>
-      </c>
-      <c r="N147" t="s">
-        <v>110</v>
-      </c>
-      <c r="O147" t="s">
-        <v>111</v>
+    <row r="147" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="148" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
-        <v>410</v>
-      </c>
       <c r="E148" t="s">
-        <v>411</v>
+        <v>336</v>
       </c>
       <c r="H148" t="s">
-        <v>412</v>
+        <v>337</v>
       </c>
       <c r="M148" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="N148" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="O148" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
     </row>
     <row r="149" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="E149" t="s">
-        <v>186</v>
+        <v>411</v>
       </c>
       <c r="H149" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="M149" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="N149" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="O149" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
     <row r="150" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
-        <v>225</v>
-      </c>
       <c r="E150" t="s">
-        <v>226</v>
+        <v>411</v>
+      </c>
+      <c r="H150" t="s">
+        <v>412</v>
+      </c>
+      <c r="M150" t="s">
+        <v>43</v>
+      </c>
+      <c r="N150" t="s">
+        <v>44</v>
+      </c>
+      <c r="O150" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="151" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>417</v>
+      </c>
       <c r="E151" t="s">
-        <v>336</v>
+        <v>418</v>
       </c>
       <c r="H151" t="s">
-        <v>337</v>
+        <v>418</v>
       </c>
       <c r="M151" t="s">
-        <v>43</v>
+        <v>486</v>
       </c>
       <c r="N151" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="O151" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
     </row>
     <row r="152" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E152" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
       <c r="H152" t="s">
-        <v>412</v>
+        <v>418</v>
       </c>
       <c r="M152" t="s">
-        <v>79</v>
+        <v>486</v>
       </c>
       <c r="N152" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="O152" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="E153" t="s">
-        <v>411</v>
-      </c>
-      <c r="H153" t="s">
-        <v>412</v>
-      </c>
-      <c r="M153" t="s">
-        <v>43</v>
-      </c>
-      <c r="N153" t="s">
-        <v>44</v>
-      </c>
-      <c r="O153" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A154" t="s">
-        <v>417</v>
-      </c>
-      <c r="E154" t="s">
-        <v>418</v>
-      </c>
-      <c r="H154" t="s">
-        <v>418</v>
-      </c>
-      <c r="M154" t="s">
-        <v>489</v>
-      </c>
-      <c r="N154" t="s">
-        <v>19</v>
-      </c>
-      <c r="O154" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="H153" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="I153" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="M153" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N153" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O153" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A154" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="H154" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="M154" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N154" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O154" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="155" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>417</v>
+        <v>425</v>
       </c>
       <c r="E155" t="s">
-        <v>418</v>
+        <v>186</v>
       </c>
       <c r="H155" t="s">
-        <v>418</v>
+        <v>187</v>
       </c>
       <c r="M155" t="s">
-        <v>489</v>
+        <v>100</v>
       </c>
       <c r="N155" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
       <c r="O155" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="156" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A156" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="F156" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="H156" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="I156" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="M156" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N156" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="O156" s="1" t="s">
-        <v>39</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E156" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="H156" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="M156" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="N156" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="O156" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="157" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>422</v>
+        <v>338</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>423</v>
+        <v>339</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>340</v>
       </c>
       <c r="H157" s="1" t="s">
-        <v>424</v>
+        <v>341</v>
       </c>
       <c r="M157" s="1" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="N157" s="1" t="s">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="O157" s="1" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
     </row>
     <row r="158" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="E158" t="s">
-        <v>186</v>
+        <v>427</v>
       </c>
       <c r="H158" t="s">
-        <v>187</v>
+        <v>428</v>
       </c>
       <c r="M158" t="s">
-        <v>100</v>
-      </c>
-      <c r="N158" t="s">
-        <v>101</v>
-      </c>
-      <c r="O158" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="159" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A159" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="E159" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="H159" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="M159" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="159" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A159" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="H159" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="M159" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="160" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>426</v>
+      </c>
+      <c r="E160" t="s">
+        <v>414</v>
+      </c>
+      <c r="H160" t="s">
+        <v>415</v>
+      </c>
+      <c r="M160" t="s">
         <v>91</v>
       </c>
-      <c r="N159" s="2" t="s">
+      <c r="N160" t="s">
         <v>92</v>
       </c>
-      <c r="O159" s="2" t="s">
+      <c r="O160" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="160" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A160" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="F160" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="H160" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="M160" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="N160" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O160" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="161" spans="1:15" x14ac:dyDescent="0.2">
@@ -4977,971 +4956,808 @@
         <v>426</v>
       </c>
       <c r="E161" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="H161" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="M161" t="s">
-        <v>32</v>
+        <v>94</v>
+      </c>
+      <c r="N161" t="s">
+        <v>95</v>
+      </c>
+      <c r="O161" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="162" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>324</v>
+        <v>97</v>
       </c>
       <c r="E162" t="s">
-        <v>325</v>
+        <v>98</v>
       </c>
       <c r="H162" t="s">
-        <v>326</v>
+        <v>99</v>
       </c>
       <c r="M162" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A163" t="s">
-        <v>426</v>
-      </c>
-      <c r="E163" t="s">
-        <v>414</v>
-      </c>
-      <c r="H163" t="s">
-        <v>415</v>
-      </c>
-      <c r="M163" t="s">
+        <v>86</v>
+      </c>
+      <c r="N162" t="s">
+        <v>87</v>
+      </c>
+      <c r="O162" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="163" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A163" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="H163" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="M163" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="N163" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="O163" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="164" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A164" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="H164" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="M164" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="N163" t="s">
+      <c r="N164" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="O163" t="s">
+      <c r="O164" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A164" t="s">
-        <v>426</v>
-      </c>
-      <c r="E164" t="s">
-        <v>414</v>
-      </c>
-      <c r="H164" t="s">
-        <v>415</v>
-      </c>
-      <c r="M164" t="s">
-        <v>94</v>
-      </c>
-      <c r="N164" t="s">
-        <v>95</v>
-      </c>
-      <c r="O164" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A165" t="s">
-        <v>97</v>
-      </c>
-      <c r="E165" t="s">
-        <v>98</v>
-      </c>
-      <c r="H165" t="s">
-        <v>99</v>
-      </c>
-      <c r="M165" t="s">
-        <v>86</v>
-      </c>
-      <c r="N165" t="s">
-        <v>87</v>
-      </c>
-      <c r="O165" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A166" t="s">
-        <v>429</v>
-      </c>
-      <c r="E166" t="s">
-        <v>430</v>
-      </c>
-      <c r="H166" t="s">
-        <v>431</v>
-      </c>
-      <c r="M166" t="s">
-        <v>86</v>
-      </c>
-      <c r="N166" t="s">
-        <v>87</v>
-      </c>
-      <c r="O166" t="s">
-        <v>88</v>
+    <row r="165" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A165" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="H165" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="M165" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N165" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O165" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="166" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A166" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="H166" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="M166" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="N166" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="O166" s="1" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="167" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>348</v>
+        <v>244</v>
       </c>
       <c r="E167" t="s">
-        <v>349</v>
+        <v>245</v>
+      </c>
+      <c r="F167" t="s">
+        <v>433</v>
       </c>
       <c r="H167" t="s">
-        <v>350</v>
+        <v>246</v>
+      </c>
+      <c r="I167" t="s">
+        <v>434</v>
       </c>
       <c r="M167" t="s">
-        <v>91</v>
-      </c>
-      <c r="N167" t="s">
-        <v>92</v>
-      </c>
-      <c r="O167" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
     </row>
     <row r="168" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>230</v>
+        <v>435</v>
       </c>
       <c r="E168" t="s">
-        <v>231</v>
+        <v>436</v>
       </c>
       <c r="H168" t="s">
-        <v>232</v>
+        <v>437</v>
       </c>
       <c r="M168" t="s">
-        <v>91</v>
-      </c>
-      <c r="N168" t="s">
-        <v>92</v>
-      </c>
-      <c r="O168" t="s">
-        <v>93</v>
+        <v>28</v>
       </c>
     </row>
     <row r="169" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>432</v>
+        <v>438</v>
       </c>
       <c r="E169" t="s">
-        <v>433</v>
+        <v>439</v>
       </c>
       <c r="H169" t="s">
-        <v>434</v>
+        <v>440</v>
       </c>
       <c r="M169" t="s">
-        <v>182</v>
+        <v>86</v>
       </c>
       <c r="N169" t="s">
-        <v>183</v>
+        <v>87</v>
       </c>
       <c r="O169" t="s">
-        <v>184</v>
+        <v>88</v>
       </c>
     </row>
     <row r="170" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>244</v>
+        <v>441</v>
       </c>
       <c r="E170" t="s">
-        <v>245</v>
-      </c>
-      <c r="F170" t="s">
-        <v>433</v>
+        <v>443</v>
       </c>
       <c r="H170" t="s">
-        <v>246</v>
-      </c>
-      <c r="I170" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="M170" t="s">
-        <v>115</v>
+        <v>33</v>
       </c>
     </row>
     <row r="171" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
       <c r="E171" t="s">
-        <v>436</v>
+        <v>445</v>
       </c>
       <c r="H171" t="s">
-        <v>437</v>
+        <v>446</v>
       </c>
       <c r="M171" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A172" t="s">
-        <v>438</v>
-      </c>
-      <c r="E172" t="s">
-        <v>439</v>
-      </c>
-      <c r="H172" t="s">
-        <v>440</v>
-      </c>
-      <c r="M172" t="s">
-        <v>86</v>
-      </c>
-      <c r="N172" t="s">
-        <v>87</v>
-      </c>
-      <c r="O172" t="s">
-        <v>88</v>
+        <v>116</v>
+      </c>
+      <c r="N171" t="s">
+        <v>117</v>
+      </c>
+      <c r="O171" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="172" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="H172" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="M172" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N172" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O172" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="173" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>441</v>
+        <v>122</v>
       </c>
       <c r="E173" t="s">
-        <v>443</v>
+        <v>123</v>
       </c>
       <c r="H173" t="s">
-        <v>442</v>
+        <v>124</v>
       </c>
       <c r="M173" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A174" t="s">
-        <v>444</v>
-      </c>
-      <c r="E174" t="s">
-        <v>445</v>
-      </c>
-      <c r="H174" t="s">
-        <v>446</v>
-      </c>
-      <c r="M174" t="s">
-        <v>116</v>
-      </c>
-      <c r="N174" t="s">
-        <v>117</v>
-      </c>
-      <c r="O174" t="s">
-        <v>118</v>
+        <v>94</v>
+      </c>
+      <c r="N173" t="s">
+        <v>95</v>
+      </c>
+      <c r="O173" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="174" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A174" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="M174" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="175" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>447</v>
+        <v>130</v>
       </c>
       <c r="E175" t="s">
-        <v>448</v>
+        <v>131</v>
       </c>
       <c r="H175" t="s">
-        <v>449</v>
+        <v>132</v>
       </c>
       <c r="M175" t="s">
-        <v>43</v>
+        <v>161</v>
       </c>
       <c r="N175" t="s">
-        <v>44</v>
+        <v>162</v>
       </c>
       <c r="O175" t="s">
-        <v>45</v>
+        <v>163</v>
       </c>
     </row>
     <row r="176" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="E176" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="H176" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="M176" t="s">
-        <v>94</v>
-      </c>
-      <c r="N176" t="s">
-        <v>95</v>
-      </c>
-      <c r="O176" t="s">
-        <v>96</v>
+        <v>133</v>
       </c>
     </row>
     <row r="177" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>450</v>
+        <v>130</v>
       </c>
       <c r="E177" t="s">
-        <v>451</v>
+        <v>131</v>
+      </c>
+      <c r="H177" t="s">
+        <v>132</v>
       </c>
       <c r="M177" t="s">
-        <v>52</v>
+        <v>182</v>
+      </c>
+      <c r="N177" t="s">
+        <v>183</v>
+      </c>
+      <c r="O177" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="178" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="E178" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="H178" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="M178" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="N178" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="O178" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
     <row r="179" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="E179" t="s">
-        <v>131</v>
+        <v>135</v>
+      </c>
+      <c r="F179" t="s">
+        <v>430</v>
       </c>
       <c r="H179" t="s">
-        <v>132</v>
+        <v>136</v>
+      </c>
+      <c r="I179" t="s">
+        <v>431</v>
       </c>
       <c r="M179" t="s">
-        <v>133</v>
+        <v>86</v>
+      </c>
+      <c r="N179" t="s">
+        <v>87</v>
+      </c>
+      <c r="O179" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="180" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="E180" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="H180" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="M180" t="s">
-        <v>182</v>
+        <v>152</v>
       </c>
       <c r="N180" t="s">
-        <v>183</v>
+        <v>153</v>
       </c>
       <c r="O180" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
     </row>
     <row r="181" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>134</v>
+        <v>452</v>
       </c>
       <c r="E181" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="H181" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="M181" t="s">
-        <v>167</v>
+        <v>43</v>
       </c>
       <c r="N181" t="s">
-        <v>168</v>
+        <v>44</v>
       </c>
       <c r="O181" t="s">
-        <v>169</v>
+        <v>45</v>
       </c>
     </row>
     <row r="182" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>134</v>
+        <v>453</v>
       </c>
       <c r="E182" t="s">
-        <v>135</v>
-      </c>
-      <c r="F182" t="s">
-        <v>430</v>
+        <v>454</v>
       </c>
       <c r="H182" t="s">
-        <v>136</v>
-      </c>
-      <c r="I182" t="s">
-        <v>431</v>
+        <v>455</v>
       </c>
       <c r="M182" t="s">
-        <v>86</v>
-      </c>
-      <c r="N182" t="s">
-        <v>87</v>
-      </c>
-      <c r="O182" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
     </row>
     <row r="183" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>138</v>
+        <v>456</v>
       </c>
       <c r="E183" t="s">
-        <v>139</v>
+        <v>457</v>
+      </c>
+      <c r="F183" t="s">
+        <v>220</v>
       </c>
       <c r="H183" t="s">
-        <v>140</v>
+        <v>458</v>
+      </c>
+      <c r="I183" t="s">
+        <v>221</v>
       </c>
       <c r="M183" t="s">
-        <v>152</v>
+        <v>94</v>
       </c>
       <c r="N183" t="s">
-        <v>153</v>
+        <v>95</v>
       </c>
       <c r="O183" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
     </row>
     <row r="184" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>17</v>
+        <v>456</v>
+      </c>
+      <c r="E184" t="s">
+        <v>457</v>
+      </c>
+      <c r="F184" t="s">
+        <v>223</v>
+      </c>
+      <c r="H184" t="s">
+        <v>458</v>
+      </c>
+      <c r="I184" t="s">
+        <v>224</v>
+      </c>
+      <c r="M184" t="s">
+        <v>127</v>
+      </c>
+      <c r="N184" t="s">
+        <v>128</v>
+      </c>
+      <c r="O184" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="185" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>18</v>
+        <v>459</v>
+      </c>
+      <c r="E185" t="s">
+        <v>460</v>
+      </c>
+      <c r="H185" t="s">
+        <v>461</v>
+      </c>
+      <c r="M185" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="186" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>22</v>
-      </c>
-      <c r="B186" t="s">
-        <v>23</v>
-      </c>
-      <c r="C186" t="s">
-        <v>24</v>
+        <v>146</v>
+      </c>
+      <c r="E186" t="s">
+        <v>147</v>
+      </c>
+      <c r="F186" t="s">
+        <v>462</v>
+      </c>
+      <c r="H186" t="s">
+        <v>148</v>
+      </c>
+      <c r="I186" t="s">
+        <v>463</v>
+      </c>
+      <c r="M186" t="s">
+        <v>100</v>
+      </c>
+      <c r="N186" t="s">
+        <v>101</v>
+      </c>
+      <c r="O186" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="187" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>452</v>
+        <v>146</v>
       </c>
       <c r="E187" t="s">
-        <v>453</v>
+        <v>463</v>
       </c>
       <c r="H187" t="s">
-        <v>454</v>
+        <v>465</v>
       </c>
       <c r="M187" t="s">
-        <v>179</v>
+        <v>94</v>
       </c>
       <c r="N187" t="s">
-        <v>180</v>
+        <v>95</v>
       </c>
       <c r="O187" t="s">
-        <v>181</v>
+        <v>96</v>
       </c>
     </row>
     <row r="188" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>466</v>
+      </c>
       <c r="E188" t="s">
-        <v>15</v>
+        <v>467</v>
       </c>
       <c r="H188" t="s">
-        <v>16</v>
+        <v>468</v>
       </c>
       <c r="M188" t="s">
-        <v>489</v>
+        <v>57</v>
       </c>
       <c r="N188" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="O188" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
     </row>
     <row r="189" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>452</v>
+        <v>469</v>
       </c>
       <c r="E189" t="s">
-        <v>453</v>
+        <v>470</v>
       </c>
       <c r="H189" t="s">
-        <v>454</v>
+        <v>471</v>
       </c>
       <c r="M189" t="s">
-        <v>119</v>
+        <v>297</v>
       </c>
       <c r="N189" t="s">
-        <v>120</v>
+        <v>298</v>
       </c>
       <c r="O189" t="s">
-        <v>121</v>
+        <v>299</v>
       </c>
     </row>
     <row r="190" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>469</v>
+      </c>
       <c r="E190" t="s">
-        <v>15</v>
+        <v>463</v>
       </c>
       <c r="H190" t="s">
-        <v>16</v>
+        <v>464</v>
       </c>
       <c r="M190" t="s">
-        <v>489</v>
+        <v>300</v>
       </c>
       <c r="N190" t="s">
-        <v>19</v>
+        <v>301</v>
       </c>
       <c r="O190" t="s">
-        <v>20</v>
+        <v>302</v>
       </c>
     </row>
     <row r="191" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>142</v>
+        <v>469</v>
       </c>
       <c r="E191" t="s">
-        <v>143</v>
+        <v>463</v>
       </c>
       <c r="H191" t="s">
-        <v>144</v>
+        <v>471</v>
       </c>
       <c r="M191" t="s">
-        <v>119</v>
+        <v>303</v>
       </c>
       <c r="N191" t="s">
-        <v>120</v>
+        <v>304</v>
       </c>
       <c r="O191" t="s">
-        <v>121</v>
+        <v>305</v>
       </c>
     </row>
     <row r="192" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>455</v>
+        <v>472</v>
       </c>
       <c r="E192" t="s">
-        <v>143</v>
+        <v>470</v>
       </c>
       <c r="H192" t="s">
-        <v>144</v>
+        <v>473</v>
       </c>
       <c r="M192" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="N192" t="s">
-        <v>44</v>
+        <v>92</v>
       </c>
       <c r="O192" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
     </row>
     <row r="193" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A193" t="s">
-        <v>456</v>
-      </c>
       <c r="E193" t="s">
-        <v>457</v>
-      </c>
-      <c r="H193" t="s">
-        <v>458</v>
-      </c>
-      <c r="M193" t="s">
-        <v>52</v>
+        <v>243</v>
       </c>
     </row>
     <row r="194" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>459</v>
+        <v>466</v>
       </c>
       <c r="E194" t="s">
-        <v>460</v>
-      </c>
-      <c r="F194" t="s">
-        <v>220</v>
+        <v>467</v>
       </c>
       <c r="H194" t="s">
-        <v>461</v>
-      </c>
-      <c r="I194" t="s">
-        <v>221</v>
+        <v>468</v>
       </c>
       <c r="M194" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="N194" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="O194" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
     </row>
     <row r="195" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>459</v>
+        <v>474</v>
       </c>
       <c r="E195" t="s">
-        <v>460</v>
-      </c>
-      <c r="F195" t="s">
-        <v>223</v>
+        <v>475</v>
       </c>
       <c r="H195" t="s">
-        <v>461</v>
-      </c>
-      <c r="I195" t="s">
-        <v>224</v>
+        <v>476</v>
       </c>
       <c r="M195" t="s">
-        <v>127</v>
+        <v>170</v>
       </c>
       <c r="N195" t="s">
-        <v>128</v>
+        <v>171</v>
       </c>
       <c r="O195" t="s">
-        <v>129</v>
+        <v>172</v>
       </c>
     </row>
     <row r="196" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>462</v>
+        <v>477</v>
       </c>
       <c r="E196" t="s">
-        <v>463</v>
+        <v>478</v>
       </c>
       <c r="H196" t="s">
-        <v>464</v>
+        <v>479</v>
       </c>
       <c r="M196" t="s">
-        <v>141</v>
+        <v>116</v>
+      </c>
+      <c r="N196" t="s">
+        <v>117</v>
+      </c>
+      <c r="O196" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="197" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>146</v>
+        <v>477</v>
       </c>
       <c r="E197" t="s">
-        <v>147</v>
-      </c>
-      <c r="F197" t="s">
-        <v>465</v>
+        <v>478</v>
       </c>
       <c r="H197" t="s">
-        <v>148</v>
-      </c>
-      <c r="I197" t="s">
-        <v>466</v>
+        <v>479</v>
       </c>
       <c r="M197" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="N197" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="O197" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
     </row>
     <row r="198" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>146</v>
+        <v>480</v>
       </c>
       <c r="E198" t="s">
-        <v>466</v>
+        <v>481</v>
       </c>
       <c r="H198" t="s">
-        <v>468</v>
+        <v>482</v>
       </c>
       <c r="M198" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="N198" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="O198" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="199" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>469</v>
+        <v>247</v>
       </c>
       <c r="E199" t="s">
-        <v>470</v>
+        <v>248</v>
+      </c>
+      <c r="F199" t="s">
+        <v>481</v>
       </c>
       <c r="H199" t="s">
-        <v>471</v>
+        <v>249</v>
+      </c>
+      <c r="I199" t="s">
+        <v>482</v>
       </c>
       <c r="M199" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="N199" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="O199" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
     </row>
     <row r="200" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>472</v>
+        <v>480</v>
       </c>
       <c r="E200" t="s">
-        <v>473</v>
+        <v>481</v>
       </c>
       <c r="H200" t="s">
-        <v>474</v>
+        <v>482</v>
       </c>
       <c r="M200" t="s">
-        <v>297</v>
+        <v>86</v>
       </c>
       <c r="N200" t="s">
-        <v>298</v>
+        <v>87</v>
       </c>
       <c r="O200" t="s">
-        <v>299</v>
+        <v>88</v>
       </c>
     </row>
     <row r="201" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>472</v>
+        <v>483</v>
       </c>
       <c r="E201" t="s">
-        <v>466</v>
+        <v>484</v>
       </c>
       <c r="H201" t="s">
-        <v>467</v>
+        <v>479</v>
       </c>
       <c r="M201" t="s">
-        <v>300</v>
+        <v>155</v>
       </c>
       <c r="N201" t="s">
-        <v>301</v>
+        <v>156</v>
       </c>
       <c r="O201" t="s">
-        <v>302</v>
+        <v>157</v>
       </c>
     </row>
     <row r="202" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>472</v>
+        <v>485</v>
       </c>
       <c r="E202" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="H202" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="M202" t="s">
-        <v>303</v>
-      </c>
-      <c r="N202" t="s">
-        <v>304</v>
-      </c>
-      <c r="O202" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A203" t="s">
-        <v>475</v>
-      </c>
-      <c r="E203" t="s">
-        <v>473</v>
-      </c>
-      <c r="H203" t="s">
-        <v>476</v>
-      </c>
-      <c r="M203" t="s">
-        <v>91</v>
-      </c>
-      <c r="N203" t="s">
-        <v>92</v>
-      </c>
-      <c r="O203" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="204" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="E204" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="205" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A205" t="s">
-        <v>469</v>
-      </c>
-      <c r="E205" t="s">
-        <v>470</v>
-      </c>
-      <c r="H205" t="s">
-        <v>471</v>
-      </c>
-      <c r="M205" t="s">
-        <v>68</v>
-      </c>
-      <c r="N205" t="s">
-        <v>69</v>
-      </c>
-      <c r="O205" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="206" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A206" t="s">
-        <v>477</v>
-      </c>
-      <c r="E206" t="s">
-        <v>478</v>
-      </c>
-      <c r="H206" t="s">
-        <v>479</v>
-      </c>
-      <c r="M206" t="s">
-        <v>170</v>
-      </c>
-      <c r="N206" t="s">
-        <v>171</v>
-      </c>
-      <c r="O206" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A207" t="s">
-        <v>480</v>
-      </c>
-      <c r="E207" t="s">
-        <v>481</v>
-      </c>
-      <c r="H207" t="s">
-        <v>482</v>
-      </c>
-      <c r="M207" t="s">
-        <v>116</v>
-      </c>
-      <c r="N207" t="s">
-        <v>117</v>
-      </c>
-      <c r="O207" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A208" t="s">
-        <v>480</v>
-      </c>
-      <c r="E208" t="s">
-        <v>481</v>
-      </c>
-      <c r="H208" t="s">
-        <v>482</v>
-      </c>
-      <c r="M208" t="s">
-        <v>116</v>
-      </c>
-      <c r="N208" t="s">
-        <v>117</v>
-      </c>
-      <c r="O208" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="209" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A209" t="s">
-        <v>483</v>
-      </c>
-      <c r="E209" t="s">
-        <v>484</v>
-      </c>
-      <c r="H209" t="s">
-        <v>485</v>
-      </c>
-      <c r="M209" t="s">
-        <v>100</v>
-      </c>
-      <c r="N209" t="s">
-        <v>101</v>
-      </c>
-      <c r="O209" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="210" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A210" t="s">
-        <v>247</v>
-      </c>
-      <c r="E210" t="s">
-        <v>248</v>
-      </c>
-      <c r="F210" t="s">
-        <v>484</v>
-      </c>
-      <c r="H210" t="s">
-        <v>249</v>
-      </c>
-      <c r="I210" t="s">
-        <v>485</v>
-      </c>
-      <c r="M210" t="s">
-        <v>86</v>
-      </c>
-      <c r="N210" t="s">
-        <v>87</v>
-      </c>
-      <c r="O210" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="211" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A211" t="s">
-        <v>483</v>
-      </c>
-      <c r="E211" t="s">
-        <v>484</v>
-      </c>
-      <c r="H211" t="s">
-        <v>485</v>
-      </c>
-      <c r="M211" t="s">
-        <v>86</v>
-      </c>
-      <c r="N211" t="s">
-        <v>87</v>
-      </c>
-      <c r="O211" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="212" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A212" t="s">
-        <v>486</v>
-      </c>
-      <c r="E212" t="s">
-        <v>487</v>
-      </c>
-      <c r="H212" t="s">
-        <v>482</v>
-      </c>
-      <c r="M212" t="s">
-        <v>155</v>
-      </c>
-      <c r="N212" t="s">
-        <v>156</v>
-      </c>
-      <c r="O212" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="213" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A213" t="s">
-        <v>488</v>
-      </c>
-      <c r="E213" t="s">
-        <v>470</v>
-      </c>
-      <c r="H213" t="s">
-        <v>471</v>
-      </c>
-      <c r="M213" t="s">
         <v>133</v>
       </c>
     </row>

</xml_diff>